<commit_message>
changes to finish app
</commit_message>
<xml_diff>
--- a/utils/Produtos_new.xlsx
+++ b/utils/Produtos_new.xlsx
@@ -485,16 +485,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>5.0341</v>
+        <v>5.0179</v>
       </c>
       <c r="E2" t="n">
-        <v>5034.049658999999</v>
+        <v>5017.849821</v>
       </c>
       <c r="F2" t="n">
         <v>1.4</v>
       </c>
       <c r="G2" t="n">
-        <v>7047.669522599998</v>
+        <v>7024.9897494</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>5.532853457000001</v>
+        <v>5.515073532000001</v>
       </c>
       <c r="E3" t="n">
-        <v>24897.8405565</v>
+        <v>24817.830894</v>
       </c>
       <c r="F3" t="n">
         <v>2</v>
       </c>
       <c r="G3" t="n">
-        <v>49795.68111300001</v>
+        <v>49635.661788</v>
       </c>
     </row>
     <row r="4">
@@ -539,16 +539,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>5.0341</v>
+        <v>5.0179</v>
       </c>
       <c r="E4" t="n">
-        <v>4530.639658999999</v>
+        <v>4516.059821</v>
       </c>
       <c r="F4" t="n">
         <v>1.7</v>
       </c>
       <c r="G4" t="n">
-        <v>7702.087420299998</v>
+        <v>7677.301695699999</v>
       </c>
     </row>
     <row r="5">
@@ -566,16 +566,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>5.0341</v>
+        <v>5.0179</v>
       </c>
       <c r="E5" t="n">
-        <v>4022.245899999999</v>
+        <v>4009.3021</v>
       </c>
       <c r="F5" t="n">
         <v>1.7</v>
       </c>
       <c r="G5" t="n">
-        <v>6837.818029999999</v>
+        <v>6815.813569999999</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>5.532853457000001</v>
+        <v>5.515073532000001</v>
       </c>
       <c r="E6" t="n">
-        <v>16598.560371</v>
+        <v>16545.220596</v>
       </c>
       <c r="F6" t="n">
         <v>1.9</v>
       </c>
       <c r="G6" t="n">
-        <v>31537.2647049</v>
+        <v>31435.9191324</v>
       </c>
     </row>
     <row r="7">
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>5.0341</v>
+        <v>5.0179</v>
       </c>
       <c r="E7" t="n">
-        <v>2418.784368</v>
+        <v>2411.000592</v>
       </c>
       <c r="F7" t="n">
         <v>2</v>
       </c>
       <c r="G7" t="n">
-        <v>4837.568736</v>
+        <v>4822.001184000001</v>
       </c>
     </row>
     <row r="8">

</xml_diff>